<commit_message>
adding tabs + changes
</commit_message>
<xml_diff>
--- a/backend/scouting-data.xlsx
+++ b/backend/scouting-data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Scouter Name</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>ff</t>
+  </si>
+  <si>
+    <t>suday</t>
+  </si>
+  <si>
+    <t>they scuk</t>
+  </si>
+  <si>
+    <t>its fine</t>
+  </si>
+  <si>
+    <t>wtv</t>
   </si>
 </sst>
 </file>
@@ -447,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,6 +564,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
added back css styles
</commit_message>
<xml_diff>
--- a/backend/scouting-data.xlsx
+++ b/backend/scouting-data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Scouter Name</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>fdsaf</t>
+  </si>
+  <si>
+    <t>qg</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t>fdsafdsa hi</t>
   </si>
 </sst>
 </file>
@@ -471,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -610,6 +619,23 @@
         <v>27</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
hosting from pc ip currently
</commit_message>
<xml_diff>
--- a/backend/scouting-data.xlsx
+++ b/backend/scouting-data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Scouter Name</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>ff</t>
+  </si>
+  <si>
+    <t>suday</t>
+  </si>
+  <si>
+    <t>cool</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
@@ -447,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,6 +564,40 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>